<commit_message>
Add the new items for the DlibIssueList20190402
Add the new items
</commit_message>
<xml_diff>
--- a/DlibIssueList20190402.xlsx
+++ b/DlibIssueList20190402.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengshuang/Documents/Programing Guide/ComputerVision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengshuang/Documents/Programing Guide/ComputerVision/GitHub/zhengshuangstar/hello-world.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>编译过程中出现：
 Error1060：C1060: compiler is out of heap space</t>
@@ -239,6 +239,39 @@
   <si>
     <t>https://github.com/takuya-takeuchi/FaceRecognitionDotNet/issues/36</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to realize in real time face detection?
+As far as I know, for python we could use "ret, frame = video_capture.read()" to get frame and input into face_locations to realize real time detect.
+For FaceRecognitionDotNet, we have to nominate the specific image path, sorry for my stupid, I tried a lot of times, still can not find a good way to input bytes or array , or transfer bytes or array into Image into FaceLocations instead of image path .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You created already BitmapSource from BitmapFrame.Create(bmp). So you can manipulate raw image data from it. Maybe you can refer the following code (Not test)
+int stride = (width  * (channels * 8 + 7)) / 8;
+var buffer = new byte[stride];
+var output = new byte[width * height * channels];
+fixed(byte* po = &amp;output[0])
+fixed(byte* pb = &amp;buffer[0])
+{
+   var p = po;
+   for (int y = 0; y &lt; height; y++)
+   {
+      roi.Y = y;
+      bitmapSource.CopyPixels(roi, (IntPtr)pb, stride, stride);
+      Marshal.Copy(pb, output, width * channels * y, width * channels)
+   }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create many face encoding data which are extracted from small face image of target person. And use them for small detected face image while matching. You can decide exact person by knn, average of all matching, etc.
+However, far face image has a tendency to occur false negative hit.
+I think it is one way to give up about low quality face image.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/takuya-takeuchi/FaceRecognitionDotNet/issues/23</t>
   </si>
 </sst>
 </file>
@@ -311,7 +344,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -325,6 +358,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -768,6 +804,24 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="320">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -776,6 +830,7 @@
     <hyperlink ref="E5" r:id="rId3"/>
     <hyperlink ref="E6" r:id="rId4"/>
     <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add the issue that .net framework4.6.1 is not compatiable with .net standard2.0
Add the issue that .net framework4.6.1 is not compatiable with .net standard2.0
</commit_message>
<xml_diff>
--- a/DlibIssueList20190402.xlsx
+++ b/DlibIssueList20190402.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>编译过程中出现：
 Error1060：C1060: compiler is out of heap space</t>
@@ -289,6 +289,31 @@
   <si>
     <t>https://docs.microsoft.com/en-us/dotnet/standard/net-standard
 https://docs.microsoft.com/en-us/dotnet/standard/net-standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.net framework4.6.1调用.net standard2.0的程序时报错，提示“System.BadImageFormatException:“试图加载格式不正确的程序。 (异常来自 HRESULT:0x8007000B)””</t>
+    <rPh sb="0" eb="2">
+      <t>diao'y</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.net framework4.6.1并未完全兼容.net standard2.0， 当项目框架换为.net framework4.7.2时不报错</t>
+    <rPh sb="0" eb="2">
+      <t>bing'wei</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目框架升级为4.7.2</t>
+    <rPh sb="0" eb="2">
+      <t>xiang'm</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/dotnet/standard/net-standard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -851,6 +876,23 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="48">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -860,6 +902,7 @@
     <hyperlink ref="E6" r:id="rId4" display="https://docs.microsoft.com/en-us/dotnet/standard/net-standard"/>
     <hyperlink ref="E7" r:id="rId5"/>
     <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add the issue of the x86 dll calling problem, and upload the x64 dll to the folder
Add the issue of the x86 dll calling problem, and upload the x64 dll to the folder
</commit_message>
<xml_diff>
--- a/DlibIssueList20190402.xlsx
+++ b/DlibIssueList20190402.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>编译过程中出现：
 Error1060：C1060: compiler is out of heap space</t>
@@ -314,6 +314,27 @@
   </si>
   <si>
     <t>https://docs.microsoft.com/en-us/dotnet/standard/net-standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行时提示“试图加载格式不正确的程序”，无法加载64位的DlibDotNetNative.dll</t>
+    <rPh sb="0" eb="1">
+      <t>wei</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程序运行输出窗口提示加载x86目录下的dll，是因为勾选了项目属性中的生成-&gt;首选32位，同时平台目标设为了Any CPU</t>
+    <rPh sb="0" eb="1">
+      <t>de</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去除首选32位</t>
+    <rPh sb="0" eb="2">
+      <t>qu'chu</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -721,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -893,6 +914,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="32">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Add the new item 11 for Directory.Exist always false
Add the new item 11 for Directory.Exist always false
</commit_message>
<xml_diff>
--- a/DlibIssueList20190402.xlsx
+++ b/DlibIssueList20190402.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>编译过程中出现：
 Error1060：C1060: compiler is out of heap space</t>
@@ -334,6 +334,40 @@
     <t>去除首选32位</t>
     <rPh sb="0" eb="2">
       <t>qu'chu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在Mac命令控制台运行Example时总是提示：
+Usage: FaceDetection [options]
+Options:
+  -h|--help       Show help information
+  -d|--directory  The directory path which includes image files
+  -c|--cpus       The number of CPU cores to use in parallel. -1 means "use all in system"
+  -m|--model      Which face detection model to use. Options are "hog" or "cnn".</t>
+    <rPh sb="0" eb="1">
+      <t>zai</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调查后应是目录无法找到，应是此处报错
+ if (!Directory.Exists(imageToCheck))
+                {
+                    app.ShowHelp();
+                    Console.WriteLine($"\n\tdirectory: {imageToCheck}");
+                    return -1;
+                }
+原因是因为目录中含有空格“Programing Guide”，在Mac控制台中空格被转化为\，即以上内容转换为“/Programing\ Guide/ComputerVision/FaceRecognitionDotNet/"，但在.net core中却无法解析此格式，在去除反斜线后即可正常读取，即“/Programing Guide/ComputerVision/FaceRecognitionDotNet/"是正常的</t>
+    <rPh sb="0" eb="2">
+      <t>diao'c</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去除文件夹名称中的空格</t>
+    <rPh sb="0" eb="2">
+      <t>qu'ch</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -742,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -928,6 +962,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="192">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Add 12 update models
</commit_message>
<xml_diff>
--- a/DlibIssueList20190402.xlsx
+++ b/DlibIssueList20190402.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengshuang/Documents/Programing Guide/ComputerVision/GitHub/zhengshuangstar/hello-world.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengshuang/Documents/ProgramingGuide/ComputerVision/GitHub/zhengshuangstar/hello-world.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>编译过程中出现：
 Error1060：C1060: compiler is out of heap space</t>
@@ -368,6 +368,29 @@
     <t>去除文件夹名称中的空格</t>
     <rPh sb="0" eb="2">
       <t>qu'ch</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当在Mac上运行FaceDetection时提示：
+ibc++abi.dylib: terminating with uncaught exception of type dlib::serialization_error: An error occurred while trying to read the first object from the file /Users/zhengshuang/Documents/ProgramingGuide/ComputerVision/FaceRecognitionDotNet/FaceRecognitionDotNet/examples/FaceDetection/models/shape_predictor_68_face_landmarks.dat.
+ERROR: Error deserializing object of type int</t>
+    <rPh sb="0" eb="35">
+      <t>dang'yun'x</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所使用Models中内容存在不正确，使用Tests项目Debug目录中的Models后变好使</t>
+    <rPh sb="0" eb="1">
+      <t>shang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换Models目录内容</t>
+    <rPh sb="0" eb="2">
+      <t>geng'h</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -776,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -976,6 +999,20 @@
         <v>41</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="144">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>